<commit_message>
add statistical result pdf file in the report
</commit_message>
<xml_diff>
--- a/statistical result.xlsx
+++ b/statistical result.xlsx
@@ -112,18 +112,18 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,11 +418,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="550304256"/>
-        <c:axId val="110139008"/>
+        <c:axId val="137361920"/>
+        <c:axId val="106862208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550304256"/>
+        <c:axId val="137361920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110139008"/>
+        <c:crossAx val="106862208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -439,7 +439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110139008"/>
+        <c:axId val="106862208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -451,7 +451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550304256"/>
+        <c:crossAx val="137361920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -798,7 +798,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -816,180 +816,180 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="L2" s="1" t="s">
+      <c r="E2" s="4"/>
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="3" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>0.6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>0.95</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>0.379</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>0.111</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="1">
         <v>1.09E-3</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="1">
         <v>0</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>0.65</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>0.85</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>0.379</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>0.13600000000000001</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="1">
         <v>1.545E-2</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="1">
         <v>2</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>0.65</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>0.95</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.111</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="1">
         <v>1.9400000000000001E-3</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="1">
         <v>1</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>0.65</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>0.95</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>0.111</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="1">
         <v>1.9400000000000001E-3</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="1">
         <v>1</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="1">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1016,7 +1016,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>